<commit_message>
Changed field titles to lowercase
</commit_message>
<xml_diff>
--- a/databases/staffDetails_L2.xlsx
+++ b/databases/staffDetails_L2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tech/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D8E52D2-AE23-AA42-B847-44F48830156C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C6D4DF-E0B4-3F4C-B72E-1DCCE15CE4BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="staffDetails_L2" sheetId="1" r:id="rId1"/>
@@ -33,30 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="205">
   <si>
-    <t>Current_Teacher</t>
-  </si>
-  <si>
-    <t>Teacher_Surname</t>
-  </si>
-  <si>
-    <t>Teacher_Christian</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Tax-30%</t>
-  </si>
-  <si>
-    <t>Super</t>
-  </si>
-  <si>
-    <t>Started</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
     <t>BRL</t>
   </si>
   <si>
@@ -490,9 +466,6 @@
     <t>Sam</t>
   </si>
   <si>
-    <t>Teacher_FormYr_1</t>
-  </si>
-  <si>
     <t>Cyphers removed (unneeded as cyphers are already stored</t>
   </si>
   <si>
@@ -544,27 +517,15 @@
     <t>Column name change</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
     <t>Missing data where required</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>Assistant Principal Year 9</t>
   </si>
   <si>
     <t>Dean Year 9</t>
   </si>
   <si>
-    <t>Subject_2</t>
-  </si>
-  <si>
     <t>&lt;-- Column split --&gt;</t>
   </si>
   <si>
@@ -619,9 +580,6 @@
     <t>Changed value type (example, string to integer)</t>
   </si>
   <si>
-    <t>YOB</t>
-  </si>
-  <si>
     <t>YOB - Year of birth</t>
   </si>
   <si>
@@ -646,7 +604,49 @@
     <t>SAE</t>
   </si>
   <si>
-    <t>Teacher_FormMentors</t>
+    <t>teacher_surname</t>
+  </si>
+  <si>
+    <t>teacher_cypher</t>
+  </si>
+  <si>
+    <t>theacher_christan</t>
+  </si>
+  <si>
+    <t>teacher_form</t>
+  </si>
+  <si>
+    <t>teacher_form_mentors</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>subject_2</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>yob</t>
+  </si>
+  <si>
+    <t>started</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>super</t>
   </si>
 </sst>
 </file>
@@ -795,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -808,8 +808,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -817,16 +815,13 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="8" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="8" fontId="1" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -834,10 +829,6 @@
     <xf numFmtId="1" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -851,8 +842,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,11 +1166,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:G1"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1185,68 +1181,68 @@
     <col min="7" max="7" width="4.1640625" customWidth="1"/>
     <col min="8" max="8" width="34.1640625" customWidth="1"/>
     <col min="10" max="10" width="23.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="36"/>
+    <col min="11" max="11" width="14.5" style="31"/>
     <col min="13" max="13" width="14.5" style="10"/>
-    <col min="16" max="16" width="3.33203125" customWidth="1"/>
-    <col min="18" max="18" width="40.83203125" customWidth="1"/>
-    <col min="19" max="19" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" customWidth="1"/>
+    <col min="17" max="17" width="40.83203125" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="43"/>
+      <c r="Q1" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>170</v>
-      </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="39"/>
-      <c r="R1" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -1254,53 +1250,49 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="40"/>
+      <c r="F2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="33"/>
       <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="K2" s="29"/>
       <c r="L2" s="1">
         <v>1990</v>
       </c>
       <c r="M2" s="1">
         <v>2016</v>
       </c>
-      <c r="N2">
-        <f xml:space="preserve"> M2 - L2</f>
-        <v>26</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="23"/>
-      <c r="R2" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="20"/>
+      <c r="Q2" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="45"/>
+      <c r="F3" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="38"/>
       <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="33">
+        <v>4</v>
+      </c>
+      <c r="K3" s="28">
         <v>1</v>
       </c>
       <c r="L3" s="1">
@@ -1309,27 +1301,23 @@
       <c r="M3" s="1">
         <v>1990</v>
       </c>
-      <c r="N3" s="10">
-        <f t="shared" ref="N3:N40" si="0" xml:space="preserve"> M3 - L3</f>
-        <v>6</v>
-      </c>
-      <c r="O3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="23"/>
-      <c r="R3" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="Q3" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>13</v>
@@ -1337,17 +1325,17 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="40"/>
+      <c r="F4" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="33"/>
       <c r="H4" s="8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>174</v>
-      </c>
-      <c r="K4" s="33">
+        <v>162</v>
+      </c>
+      <c r="K4" s="28">
         <v>2</v>
       </c>
       <c r="L4" s="1">
@@ -1356,39 +1344,35 @@
       <c r="M4" s="1">
         <v>2008</v>
       </c>
-      <c r="N4" s="10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="O4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="23"/>
-      <c r="R4" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="20"/>
+      <c r="Q4" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="45"/>
+      <c r="F5" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="38"/>
       <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="33">
+        <v>18</v>
+      </c>
+      <c r="K5" s="28">
         <v>1</v>
       </c>
       <c r="L5" s="1">
@@ -1397,27 +1381,23 @@
       <c r="M5" s="1">
         <v>2003</v>
       </c>
-      <c r="N5" s="10">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="O5" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" s="23"/>
-      <c r="R5" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="20"/>
+      <c r="Q5" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>12</v>
@@ -1425,14 +1405,14 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="40"/>
+      <c r="F6" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="33"/>
       <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="33">
+        <v>4</v>
+      </c>
+      <c r="K6" s="28">
         <v>1</v>
       </c>
       <c r="L6" s="1">
@@ -1441,27 +1421,23 @@
       <c r="M6" s="1">
         <v>2015</v>
       </c>
-      <c r="N6" s="10">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="23"/>
-      <c r="R6" s="16" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="20"/>
+      <c r="Q6" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>13</v>
@@ -1469,17 +1445,17 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="40"/>
+      <c r="F7" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="33"/>
       <c r="H7" s="8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="K7" s="33">
+        <v>165</v>
+      </c>
+      <c r="K7" s="28">
         <v>1</v>
       </c>
       <c r="L7" s="1">
@@ -1488,42 +1464,38 @@
       <c r="M7" s="1">
         <v>2015</v>
       </c>
-      <c r="N7" s="10">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="O7" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="23"/>
-      <c r="R7" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="Q7" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8">
         <v>0</v>
       </c>
-      <c r="F8" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="40"/>
+      <c r="F8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="33"/>
       <c r="H8" s="8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>175</v>
-      </c>
-      <c r="K8" s="33">
+        <v>163</v>
+      </c>
+      <c r="K8" s="28">
         <v>5</v>
       </c>
       <c r="L8" s="1">
@@ -1532,27 +1504,23 @@
       <c r="M8" s="1">
         <v>1994</v>
       </c>
-      <c r="N8" s="10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="O8" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" s="23"/>
-      <c r="R8" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="20"/>
+      <c r="Q8" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1">
         <v>12</v>
@@ -1560,14 +1528,14 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" s="45"/>
+      <c r="F9" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="38"/>
       <c r="H9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="33">
+        <v>34</v>
+      </c>
+      <c r="K9" s="28">
         <v>1</v>
       </c>
       <c r="L9" s="1">
@@ -1576,27 +1544,23 @@
       <c r="M9" s="1">
         <v>2016</v>
       </c>
-      <c r="N9" s="10">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="O9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" s="23"/>
-      <c r="R9" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="Q9" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1">
         <v>12</v>
@@ -1604,20 +1568,20 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="G10" s="47"/>
+      <c r="F10" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="40"/>
       <c r="H10" s="8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K10" s="33">
+        <v>166</v>
+      </c>
+      <c r="K10" s="28">
         <v>2</v>
       </c>
       <c r="L10" s="1">
@@ -1626,27 +1590,23 @@
       <c r="M10" s="1">
         <v>2009</v>
       </c>
-      <c r="N10" s="10">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="O10" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="23"/>
-      <c r="R10" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="20"/>
+      <c r="Q10" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>11</v>
@@ -1654,14 +1614,14 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="40"/>
+      <c r="F11" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="33"/>
       <c r="H11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="33">
+        <v>34</v>
+      </c>
+      <c r="K11" s="28">
         <v>1</v>
       </c>
       <c r="L11" s="1">
@@ -1670,39 +1630,35 @@
       <c r="M11" s="1">
         <v>1994</v>
       </c>
-      <c r="N11" s="10">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="O11" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P11" s="23"/>
-      <c r="R11" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N11" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="Q11" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
       </c>
-      <c r="F12" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="40"/>
+      <c r="F12" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="33"/>
       <c r="H12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="35">
+        <v>18</v>
+      </c>
+      <c r="K12" s="30">
         <v>1</v>
       </c>
       <c r="L12" s="1">
@@ -1711,27 +1667,23 @@
       <c r="M12" s="1">
         <v>1999</v>
       </c>
-      <c r="N12" s="10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="O12" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" s="23"/>
-      <c r="R12" s="23" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="20"/>
+      <c r="Q12" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1">
         <v>10</v>
@@ -1739,17 +1691,17 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="40"/>
+      <c r="F13" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="33"/>
       <c r="H13" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="K13" s="35">
+        <v>61</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="K13" s="30">
         <v>2</v>
       </c>
       <c r="L13" s="1">
@@ -1758,71 +1710,63 @@
       <c r="M13" s="1">
         <v>1987</v>
       </c>
-      <c r="N13" s="10">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="O13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P13" s="23"/>
-      <c r="R13" s="24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="Q13" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
       </c>
-      <c r="F14" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="40"/>
+      <c r="F14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="33"/>
       <c r="H14" s="8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>183</v>
-      </c>
-      <c r="K14" s="33">
+        <v>170</v>
+      </c>
+      <c r="K14" s="28">
         <v>6</v>
       </c>
       <c r="L14" s="1">
         <v>1977</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="25">
         <v>2013</v>
       </c>
-      <c r="N14" s="10">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="O14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="P14" s="23"/>
-      <c r="R14" s="29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N14" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="Q14" s="25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D15" s="1">
         <v>11</v>
@@ -1830,14 +1774,14 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="40"/>
+      <c r="F15" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="33"/>
       <c r="H15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="33">
+        <v>4</v>
+      </c>
+      <c r="K15" s="28">
         <v>1</v>
       </c>
       <c r="L15" s="1">
@@ -1846,24 +1790,20 @@
       <c r="M15" s="1">
         <v>2007</v>
       </c>
-      <c r="N15" s="10">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P15" s="23"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" s="20"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1">
         <v>13</v>
@@ -1871,14 +1811,14 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="47"/>
+      <c r="F16" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="40"/>
       <c r="H16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="33">
+        <v>4</v>
+      </c>
+      <c r="K16" s="28">
         <v>1</v>
       </c>
       <c r="L16" s="1">
@@ -1887,24 +1827,20 @@
       <c r="M16" s="1">
         <v>2006</v>
       </c>
-      <c r="N16" s="10">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="O16" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" s="23"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N16" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="20"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1">
         <v>12</v>
@@ -1912,14 +1848,14 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="40"/>
+      <c r="F17" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="33"/>
       <c r="H17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="33">
+        <v>61</v>
+      </c>
+      <c r="K17" s="28">
         <v>1</v>
       </c>
       <c r="L17" s="1">
@@ -1928,39 +1864,35 @@
       <c r="M17" s="1">
         <v>2003</v>
       </c>
-      <c r="N17" s="10">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="O17" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P17" s="23"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E18" s="8">
         <v>0</v>
       </c>
-      <c r="F18" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="40"/>
+      <c r="F18" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="33"/>
       <c r="H18" s="8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J18" t="s">
-        <v>184</v>
-      </c>
-      <c r="K18" s="33">
+        <v>171</v>
+      </c>
+      <c r="K18" s="28">
         <v>5</v>
       </c>
       <c r="L18" s="1">
@@ -1969,24 +1901,20 @@
       <c r="M18" s="1">
         <v>1998</v>
       </c>
-      <c r="N18" s="10">
-        <f t="shared" si="0"/>
+      <c r="N18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O18" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P18" s="23"/>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1">
         <v>12</v>
@@ -1994,14 +1922,14 @@
       <c r="E19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="45"/>
+      <c r="F19" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="38"/>
       <c r="H19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="33">
+        <v>34</v>
+      </c>
+      <c r="K19" s="28">
         <v>1</v>
       </c>
       <c r="L19" s="1">
@@ -2010,36 +1938,32 @@
       <c r="M19" s="1">
         <v>1995</v>
       </c>
-      <c r="N19" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P19" s="23"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E20" s="8">
         <v>0</v>
       </c>
-      <c r="F20" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="G20" s="45"/>
+      <c r="F20" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="38"/>
       <c r="H20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="33">
+        <v>4</v>
+      </c>
+      <c r="K20" s="28">
         <v>1</v>
       </c>
       <c r="L20" s="1">
@@ -2048,34 +1972,30 @@
       <c r="M20" s="1">
         <v>1986</v>
       </c>
-      <c r="N20" s="10">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="O20" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P20" s="23"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E21" s="8">
         <v>0</v>
       </c>
-      <c r="F21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="40"/>
+      <c r="F21" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="33"/>
       <c r="H21" s="2"/>
-      <c r="K21" s="33">
+      <c r="K21" s="28">
         <v>3</v>
       </c>
       <c r="L21" s="1">
@@ -2084,24 +2004,20 @@
       <c r="M21" s="1">
         <v>1995</v>
       </c>
-      <c r="N21" s="10">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="P21" s="23"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N21" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D22" s="1">
         <v>11</v>
@@ -2109,14 +2025,14 @@
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="F22" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="40"/>
+      <c r="F22" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="33"/>
       <c r="H22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K22" s="33">
+        <v>34</v>
+      </c>
+      <c r="K22" s="28">
         <v>1</v>
       </c>
       <c r="L22" s="1">
@@ -2125,24 +2041,20 @@
       <c r="M22" s="1">
         <v>1982</v>
       </c>
-      <c r="N22" s="10">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="O22" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P22" s="23"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D23" s="1">
         <v>10</v>
@@ -2150,17 +2062,17 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="G23" s="46"/>
+      <c r="F23" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G23" s="39"/>
       <c r="H23" s="8" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="I23" t="s">
-        <v>186</v>
-      </c>
-      <c r="K23" s="33">
+        <v>173</v>
+      </c>
+      <c r="K23" s="28">
         <v>1</v>
       </c>
       <c r="L23" s="1">
@@ -2169,39 +2081,35 @@
       <c r="M23" s="1">
         <v>1980</v>
       </c>
-      <c r="N23" s="10">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="O23" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P23" s="23"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E24" s="8">
         <v>0</v>
       </c>
-      <c r="F24" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="40"/>
+      <c r="F24" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="33"/>
       <c r="H24" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J24" t="s">
-        <v>187</v>
-      </c>
-      <c r="K24" s="33">
+        <v>174</v>
+      </c>
+      <c r="K24" s="28">
         <v>6</v>
       </c>
       <c r="L24" s="1">
@@ -2210,24 +2118,20 @@
       <c r="M24" s="1">
         <v>1998</v>
       </c>
-      <c r="N24" s="10">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="O24" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P24" s="23"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N24" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1">
         <v>10</v>
@@ -2235,14 +2139,14 @@
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="40"/>
+      <c r="F25" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="33"/>
       <c r="H25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K25" s="33">
+        <v>89</v>
+      </c>
+      <c r="K25" s="28">
         <v>1</v>
       </c>
       <c r="L25" s="1">
@@ -2251,42 +2155,38 @@
       <c r="M25" s="1">
         <v>2012</v>
       </c>
-      <c r="N25" s="10">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="O25" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P25" s="23"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N25" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E26" s="8">
         <v>0</v>
       </c>
-      <c r="F26" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="G26" s="40"/>
+      <c r="F26" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" s="33"/>
       <c r="H26" s="8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="J26" t="s">
-        <v>188</v>
-      </c>
-      <c r="K26" s="33">
+        <v>175</v>
+      </c>
+      <c r="K26" s="28">
         <v>7</v>
       </c>
       <c r="L26" s="1">
@@ -2295,24 +2195,20 @@
       <c r="M26" s="1">
         <v>2010</v>
       </c>
-      <c r="N26" s="10">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P26" s="23"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N26" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D27" s="1">
         <v>9</v>
@@ -2320,38 +2216,34 @@
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="40"/>
+      <c r="F27" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" s="33"/>
       <c r="H27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K27" s="34"/>
+        <v>34</v>
+      </c>
+      <c r="K27" s="29"/>
       <c r="L27" s="1">
         <v>1966</v>
       </c>
       <c r="M27" s="1">
         <v>2009</v>
       </c>
-      <c r="N27" s="10">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="O27" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P27" s="23"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N27" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
@@ -2359,14 +2251,14 @@
       <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="G28" s="40"/>
+      <c r="F28" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="33"/>
       <c r="H28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="33">
+        <v>34</v>
+      </c>
+      <c r="K28" s="28">
         <v>1</v>
       </c>
       <c r="L28" s="1">
@@ -2375,36 +2267,32 @@
       <c r="M28" s="1">
         <v>2006</v>
       </c>
-      <c r="N28" s="10">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="O28" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P28" s="23"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N28" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E29" s="8">
         <v>0</v>
       </c>
-      <c r="F29" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="G29" s="40"/>
+      <c r="F29" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="33"/>
       <c r="H29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K29" s="33">
+        <v>104</v>
+      </c>
+      <c r="K29" s="28">
         <v>1</v>
       </c>
       <c r="L29" s="1">
@@ -2413,24 +2301,20 @@
       <c r="M29" s="1">
         <v>1986</v>
       </c>
-      <c r="N29" s="10">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="O29" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="P29" s="23"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N29" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D30" s="1">
         <v>12</v>
@@ -2438,17 +2322,17 @@
       <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="G30" s="40"/>
+      <c r="F30" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="33"/>
       <c r="H30" s="8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>190</v>
-      </c>
-      <c r="K30" s="33">
+        <v>177</v>
+      </c>
+      <c r="K30" s="28">
         <v>1</v>
       </c>
       <c r="L30" s="1">
@@ -2457,24 +2341,20 @@
       <c r="M30" s="1">
         <v>1993</v>
       </c>
-      <c r="N30" s="10">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="O30" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P30" s="23"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N30" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D31" s="1">
         <v>10</v>
@@ -2482,14 +2362,14 @@
       <c r="E31" s="1">
         <v>1</v>
       </c>
-      <c r="F31" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="40"/>
+      <c r="F31" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="33"/>
       <c r="H31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K31" s="33">
+        <v>34</v>
+      </c>
+      <c r="K31" s="28">
         <v>1</v>
       </c>
       <c r="L31" s="1">
@@ -2498,36 +2378,32 @@
       <c r="M31" s="1">
         <v>2001</v>
       </c>
-      <c r="N31" s="10">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="O31" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P31" s="23"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="23" t="s">
-        <v>203</v>
+      <c r="N31" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E32" s="8">
         <v>0</v>
       </c>
-      <c r="F32" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="40"/>
+      <c r="F32" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="33"/>
       <c r="H32" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K32" s="33">
+        <v>114</v>
+      </c>
+      <c r="K32" s="28">
         <v>1</v>
       </c>
       <c r="L32" s="1">
@@ -2536,36 +2412,32 @@
       <c r="M32" s="1">
         <v>1982</v>
       </c>
-      <c r="N32" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O32" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N32" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E33" s="8">
         <v>0</v>
       </c>
-      <c r="F33" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="G33" s="40"/>
+      <c r="F33" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="33"/>
       <c r="H33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="33">
+        <v>4</v>
+      </c>
+      <c r="K33" s="28">
         <v>1</v>
       </c>
       <c r="L33" s="1">
@@ -2574,24 +2446,20 @@
       <c r="M33" s="1">
         <v>1993</v>
       </c>
-      <c r="N33" s="10">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="O33" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N33" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D34" s="1">
         <v>9</v>
@@ -2599,14 +2467,14 @@
       <c r="E34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34" s="40"/>
+      <c r="F34" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G34" s="33"/>
       <c r="H34" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K34" s="33">
+        <v>123</v>
+      </c>
+      <c r="K34" s="28">
         <v>4</v>
       </c>
       <c r="L34" s="1">
@@ -2615,36 +2483,32 @@
       <c r="M34" s="1">
         <v>2014</v>
       </c>
-      <c r="N34" s="10">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="O34" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P34" s="23"/>
-    </row>
-    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N34" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E35" s="8">
         <v>0</v>
       </c>
-      <c r="F35" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="K35" s="33">
+      <c r="F35" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="G35" s="37"/>
+      <c r="H35" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="K35" s="28">
         <v>1</v>
       </c>
       <c r="L35" s="1">
@@ -2653,24 +2517,20 @@
       <c r="M35" s="1">
         <v>2011</v>
       </c>
-      <c r="N35" s="10">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="O35" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P35" s="23"/>
-    </row>
-    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N35" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D36" s="1">
         <v>9</v>
@@ -2678,76 +2538,68 @@
       <c r="E36" s="1">
         <v>1</v>
       </c>
-      <c r="F36" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="G36" s="40"/>
+      <c r="F36" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="33"/>
       <c r="H36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K36" s="33">
-        <v>1</v>
-      </c>
-      <c r="L36" s="29">
+        <v>61</v>
+      </c>
+      <c r="K36" s="28">
+        <v>1</v>
+      </c>
+      <c r="L36" s="25">
         <v>1964</v>
       </c>
       <c r="M36" s="1">
         <v>2002</v>
       </c>
-      <c r="N36" s="10">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="O36" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="P36" s="23"/>
-    </row>
-    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N36" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E37" s="8">
         <v>0</v>
       </c>
-      <c r="F37" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="G37" s="40"/>
+      <c r="F37" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37" s="33"/>
       <c r="H37" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K37" s="34"/>
+        <v>136</v>
+      </c>
+      <c r="K37" s="29"/>
       <c r="L37" s="1">
         <v>1968</v>
       </c>
       <c r="M37" s="1">
         <v>2012</v>
       </c>
-      <c r="N37" s="10">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="O37" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P37" s="23"/>
-    </row>
-    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N37" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D38" s="1">
         <v>9</v>
@@ -2756,13 +2608,13 @@
         <v>1</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K38" s="33">
+        <v>4</v>
+      </c>
+      <c r="K38" s="28">
         <v>1</v>
       </c>
       <c r="L38" s="1">
@@ -2771,36 +2623,32 @@
       <c r="M38" s="1">
         <v>1986</v>
       </c>
-      <c r="N38" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="O38" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="P38" s="23"/>
-    </row>
-    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N38" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>33</v>
+        <v>140</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="E39" s="8">
         <v>0</v>
       </c>
-      <c r="F39" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G39" s="40"/>
+      <c r="F39" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="33"/>
       <c r="H39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K39" s="33">
+        <v>141</v>
+      </c>
+      <c r="K39" s="28">
         <v>1</v>
       </c>
       <c r="L39" s="1">
@@ -2809,36 +2657,32 @@
       <c r="M39" s="1">
         <v>1993</v>
       </c>
-      <c r="N39" s="10">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="O39" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="P39" s="23"/>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N39" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" s="20"/>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E40" s="8">
         <v>0</v>
       </c>
-      <c r="F40" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="G40" s="40"/>
+      <c r="F40" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="33"/>
       <c r="H40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K40" s="33">
+        <v>61</v>
+      </c>
+      <c r="K40" s="28">
         <v>1</v>
       </c>
       <c r="L40" s="1">
@@ -2847,66 +2691,58 @@
       <c r="M40" s="1">
         <v>1981</v>
       </c>
-      <c r="N40" s="10">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="O40" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P40" s="23"/>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D41" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="48"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="N41" s="10"/>
-    </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D42" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="48"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="N40" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O40" s="20"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D41" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="41"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D42" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" s="41"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
       <c r="L42" s="7" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="M42" s="7"/>
     </row>
-    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K43" s="37"/>
-      <c r="L43" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="L45" s="38"/>
-      <c r="M45" s="38"/>
-      <c r="N45" s="38"/>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="L46" s="38"/>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
+    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K43" s="32"/>
+      <c r="L43" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="M43" s="45"/>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L44" s="45"/>
+      <c r="M44" s="45"/>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L45" s="45"/>
+      <c r="M45" s="45"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="L43:M46"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="F1:G1"/>
@@ -2937,8 +2773,7 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="L43:N46"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="F41:G41"/>
@@ -2962,121 +2797,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D51A4AB-EBA6-E24D-899D-2293B78CD359}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>5</v>
+        <v>188</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="26">
         <v>75000</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="27">
         <v>22500</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="27">
         <v>7500</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="26">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="26">
         <v>90000</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="27">
         <v>27000</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="27">
         <v>9000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="26">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="26">
         <v>110000</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="27">
         <v>33000</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="27">
         <v>11000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="26">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="26">
         <v>55000</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="27">
         <v>16500</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="27">
         <v>5500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="26">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="26">
         <v>80000</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="27">
         <v>24000</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="27">
         <v>8000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="26">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>95000</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="18">
         <v>28500</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="18">
         <v>9500</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="26">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>65000</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <v>19500</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <v>6500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more tables & lowercased all table titles
</commit_message>
<xml_diff>
--- a/databases/staffDetails_L2.xlsx
+++ b/databases/staffDetails_L2.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tech/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C6D4DF-E0B4-3F4C-B72E-1DCCE15CE4BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55DD525-D526-1145-B13E-C2BAFD7D0264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="staffDetails_L2" sheetId="1" r:id="rId1"/>
-    <sheet name="Incomes" sheetId="2" r:id="rId2"/>
+    <sheet name="teachers" sheetId="1" r:id="rId1"/>
+    <sheet name="subjects" sheetId="4" r:id="rId2"/>
+    <sheet name="rooms" sheetId="3" r:id="rId3"/>
+    <sheet name="incomes" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1168,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -2794,10 +2796,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF96148D-3054-3446-B33B-11438D8AC45D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069431B2-E190-0A4A-AD7A-67EB2654937C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D51A4AB-EBA6-E24D-899D-2293B78CD359}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved subject data into subjects table
</commit_message>
<xml_diff>
--- a/databases/staffDetails_L2.xlsx
+++ b/databases/staffDetails_L2.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tech/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55DD525-D526-1145-B13E-C2BAFD7D0264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA12A59-5649-2A40-956E-B2A66382B570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="203">
   <si>
     <t>BRL</t>
   </si>
@@ -302,10 +302,6 @@
     <t>C3</t>
   </si>
   <si>
-    <t>English
-Drama</t>
-  </si>
-  <si>
     <t>PZK</t>
   </si>
   <si>
@@ -348,9 +344,6 @@
     <t>A9</t>
   </si>
   <si>
-    <t>arts</t>
-  </si>
-  <si>
     <t>RRA</t>
   </si>
   <si>
@@ -405,9 +398,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>Technology Transition</t>
-  </si>
-  <si>
     <t>SKA</t>
   </si>
   <si>
@@ -444,9 +434,6 @@
     <t>A6</t>
   </si>
   <si>
-    <t>ARTS</t>
-  </si>
-  <si>
     <t>TSM</t>
   </si>
   <si>
@@ -534,15 +521,9 @@
     <t>Drama</t>
   </si>
   <si>
-    <t>HOD English</t>
-  </si>
-  <si>
     <t>Learner Support</t>
   </si>
   <si>
-    <t>HOD Digital Technology</t>
-  </si>
-  <si>
     <t>General spelling correction</t>
   </si>
   <si>
@@ -552,9 +533,6 @@
     <t>Dean Year 10</t>
   </si>
   <si>
-    <t>Enlish</t>
-  </si>
-  <si>
     <t>Transition</t>
   </si>
   <si>
@@ -567,9 +545,6 @@
     <t>Science</t>
   </si>
   <si>
-    <t>Langages</t>
-  </si>
-  <si>
     <t>T6</t>
   </si>
   <si>
@@ -649,6 +624,24 @@
   </si>
   <si>
     <t>super</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Moved data to correct positon</t>
+  </si>
+  <si>
+    <t>HOD 1</t>
+  </si>
+  <si>
+    <t>HOD Digital 3</t>
+  </si>
+  <si>
+    <t>Languages</t>
   </si>
 </sst>
 </file>
@@ -693,7 +686,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -784,6 +777,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -797,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -822,8 +821,8 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="1" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="8" fontId="1" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -851,6 +850,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1165,14 +1173,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1181,7 +1189,7 @@
     <col min="4" max="5" width="22.1640625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="4.1640625" customWidth="1"/>
-    <col min="8" max="8" width="34.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
     <col min="10" max="10" width="23.83203125" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="31"/>
     <col min="13" max="13" width="14.5" style="10"/>
@@ -1192,48 +1200,48 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="42" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G1" s="43"/>
       <c r="H1" s="42" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="O1" s="43"/>
       <c r="Q1" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1256,8 +1264,8 @@
         <v>3</v>
       </c>
       <c r="G2" s="33"/>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
+      <c r="H2" s="1">
+        <v>1</v>
       </c>
       <c r="K2" s="29"/>
       <c r="L2" s="1">
@@ -1271,7 +1279,7 @@
       </c>
       <c r="O2" s="20"/>
       <c r="Q2" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1288,11 +1296,11 @@
         <v>0</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
+      <c r="H3" s="1">
+        <v>1</v>
       </c>
       <c r="K3" s="28">
         <v>1</v>
@@ -1308,7 +1316,7 @@
       </c>
       <c r="O3" s="20"/>
       <c r="Q3" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1331,11 +1339,11 @@
         <v>13</v>
       </c>
       <c r="G4" s="33"/>
-      <c r="H4" s="8" t="s">
-        <v>34</v>
+      <c r="H4" s="8">
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K4" s="28">
         <v>2</v>
@@ -1351,7 +1359,7 @@
       </c>
       <c r="O4" s="20"/>
       <c r="Q4" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1368,11 +1376,11 @@
         <v>0</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G5" s="38"/>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
+      <c r="H5" s="1">
+        <v>3</v>
       </c>
       <c r="K5" s="28">
         <v>1</v>
@@ -1388,7 +1396,7 @@
       </c>
       <c r="O5" s="20"/>
       <c r="Q5" s="13" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1411,8 +1419,8 @@
         <v>22</v>
       </c>
       <c r="G6" s="33"/>
-      <c r="H6" s="1" t="s">
-        <v>4</v>
+      <c r="H6" s="1">
+        <v>1</v>
       </c>
       <c r="K6" s="28">
         <v>1</v>
@@ -1428,7 +1436,7 @@
       </c>
       <c r="O6" s="20"/>
       <c r="Q6" s="14" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1451,11 +1459,11 @@
         <v>26</v>
       </c>
       <c r="G7" s="33"/>
-      <c r="H7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>165</v>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
       </c>
       <c r="K7" s="28">
         <v>1</v>
@@ -1471,7 +1479,7 @@
       </c>
       <c r="O7" s="20"/>
       <c r="Q7" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1491,11 +1499,11 @@
         <v>30</v>
       </c>
       <c r="G8" s="33"/>
-      <c r="H8" s="8" t="s">
-        <v>34</v>
+      <c r="H8" s="8">
+        <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K8" s="28">
         <v>5</v>
@@ -1511,7 +1519,7 @@
       </c>
       <c r="O8" s="20"/>
       <c r="Q8" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1531,11 +1539,11 @@
         <v>0</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G9" s="38"/>
-      <c r="H9" s="1" t="s">
-        <v>34</v>
+      <c r="H9" s="1">
+        <v>2</v>
       </c>
       <c r="K9" s="28">
         <v>1</v>
@@ -1551,7 +1559,7 @@
       </c>
       <c r="O9" s="20"/>
       <c r="Q9" s="12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1571,17 +1579,17 @@
         <v>0</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G10" s="40"/>
-      <c r="H10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>167</v>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>11</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="K10" s="28">
         <v>2</v>
@@ -1597,7 +1605,7 @@
       </c>
       <c r="O10" s="20"/>
       <c r="Q10" s="16" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1620,8 +1628,8 @@
         <v>41</v>
       </c>
       <c r="G11" s="33"/>
-      <c r="H11" s="1" t="s">
-        <v>34</v>
+      <c r="H11" s="1">
+        <v>2</v>
       </c>
       <c r="K11" s="28">
         <v>1</v>
@@ -1637,7 +1645,7 @@
       </c>
       <c r="O11" s="20"/>
       <c r="Q11" s="19" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1648,7 +1656,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -1657,8 +1665,8 @@
         <v>44</v>
       </c>
       <c r="G12" s="33"/>
-      <c r="H12" s="1" t="s">
-        <v>18</v>
+      <c r="H12" s="1">
+        <v>3</v>
       </c>
       <c r="K12" s="30">
         <v>1</v>
@@ -1674,7 +1682,7 @@
       </c>
       <c r="O12" s="20"/>
       <c r="Q12" s="20" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1697,11 +1705,11 @@
         <v>48</v>
       </c>
       <c r="G13" s="33"/>
-      <c r="H13" s="8" t="s">
-        <v>61</v>
+      <c r="H13" s="8">
+        <v>4</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="K13" s="30">
         <v>2</v>
@@ -1717,7 +1725,7 @@
       </c>
       <c r="O13" s="20"/>
       <c r="Q13" s="21" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1737,11 +1745,11 @@
         <v>13</v>
       </c>
       <c r="G14" s="33"/>
-      <c r="H14" s="8" t="s">
-        <v>4</v>
+      <c r="H14" s="8">
+        <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K14" s="28">
         <v>6</v>
@@ -1749,15 +1757,15 @@
       <c r="L14" s="1">
         <v>1977</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="24">
         <v>2013</v>
       </c>
       <c r="N14" s="22" t="s">
         <v>5</v>
       </c>
       <c r="O14" s="20"/>
-      <c r="Q14" s="25" t="s">
-        <v>187</v>
+      <c r="Q14" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1768,7 +1776,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1">
         <v>11</v>
@@ -1780,8 +1788,8 @@
         <v>54</v>
       </c>
       <c r="G15" s="33"/>
-      <c r="H15" s="1" t="s">
-        <v>4</v>
+      <c r="H15" s="1">
+        <v>1</v>
       </c>
       <c r="K15" s="28">
         <v>1</v>
@@ -1796,6 +1804,9 @@
         <v>9</v>
       </c>
       <c r="O15" s="20"/>
+      <c r="Q15" s="50" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
@@ -1817,8 +1828,8 @@
         <v>26</v>
       </c>
       <c r="G16" s="40"/>
-      <c r="H16" s="1" t="s">
-        <v>4</v>
+      <c r="H16" s="1">
+        <v>1</v>
       </c>
       <c r="K16" s="28">
         <v>1</v>
@@ -1854,8 +1865,8 @@
         <v>54</v>
       </c>
       <c r="G17" s="33"/>
-      <c r="H17" s="1" t="s">
-        <v>61</v>
+      <c r="H17" s="1">
+        <v>4</v>
       </c>
       <c r="K17" s="28">
         <v>1</v>
@@ -1888,11 +1899,11 @@
         <v>65</v>
       </c>
       <c r="G18" s="33"/>
-      <c r="H18" s="8" t="s">
-        <v>34</v>
+      <c r="H18" s="8">
+        <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K18" s="28">
         <v>5</v>
@@ -1925,11 +1936,11 @@
         <v>0</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G19" s="38"/>
-      <c r="H19" s="1" t="s">
-        <v>34</v>
+      <c r="H19" s="1">
+        <v>2</v>
       </c>
       <c r="K19" s="28">
         <v>1</v>
@@ -1959,11 +1970,11 @@
         <v>0</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G20" s="38"/>
-      <c r="H20" s="1" t="s">
-        <v>4</v>
+      <c r="H20" s="1">
+        <v>1</v>
       </c>
       <c r="K20" s="28">
         <v>1</v>
@@ -2031,9 +2042,10 @@
         <v>78</v>
       </c>
       <c r="G22" s="33"/>
-      <c r="H22" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="H22" s="47">
+        <v>2</v>
+      </c>
+      <c r="I22" s="48"/>
       <c r="K22" s="28">
         <v>1</v>
       </c>
@@ -2065,14 +2077,14 @@
         <v>1</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G23" s="39"/>
-      <c r="H23" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" t="s">
-        <v>173</v>
+      <c r="H23" s="8">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
       </c>
       <c r="K23" s="28">
         <v>1</v>
@@ -2105,11 +2117,11 @@
         <v>13</v>
       </c>
       <c r="G24" s="33"/>
-      <c r="H24" s="8" t="s">
-        <v>61</v>
+      <c r="H24" s="8">
+        <v>4</v>
       </c>
       <c r="J24" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K24" s="28">
         <v>6</v>
@@ -2145,8 +2157,11 @@
         <v>88</v>
       </c>
       <c r="G25" s="33"/>
-      <c r="H25" s="1" t="s">
-        <v>89</v>
+      <c r="H25" s="8">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5</v>
       </c>
       <c r="K25" s="28">
         <v>1</v>
@@ -2164,29 +2179,29 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="E26" s="8">
         <v>0</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G26" s="33"/>
-      <c r="H26" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>176</v>
+      <c r="H26" s="8">
+        <v>2</v>
+      </c>
+      <c r="I26" s="7">
+        <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K26" s="28">
         <v>7</v>
@@ -2204,13 +2219,13 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D27" s="1">
         <v>9</v>
@@ -2219,11 +2234,11 @@
         <v>1</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G27" s="33"/>
-      <c r="H27" s="1" t="s">
-        <v>34</v>
+      <c r="H27" s="1">
+        <v>2</v>
       </c>
       <c r="K27" s="29"/>
       <c r="L27" s="1">
@@ -2239,13 +2254,13 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
@@ -2254,11 +2269,11 @@
         <v>1</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28" s="33"/>
-      <c r="H28" s="1" t="s">
-        <v>34</v>
+      <c r="H28" s="8">
+        <v>2</v>
       </c>
       <c r="K28" s="28">
         <v>1</v>
@@ -2276,23 +2291,23 @@
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E29" s="8">
         <v>0</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G29" s="33"/>
-      <c r="H29" s="1" t="s">
-        <v>104</v>
+      <c r="H29" s="49">
+        <v>6</v>
       </c>
       <c r="K29" s="28">
         <v>1</v>
@@ -2310,13 +2325,13 @@
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D30" s="1">
         <v>12</v>
@@ -2325,14 +2340,14 @@
         <v>0</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G30" s="33"/>
-      <c r="H30" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" t="s">
-        <v>177</v>
+      <c r="H30" s="8">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>9</v>
       </c>
       <c r="K30" s="28">
         <v>1</v>
@@ -2350,13 +2365,13 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D31" s="1">
         <v>10</v>
@@ -2368,8 +2383,8 @@
         <v>30</v>
       </c>
       <c r="G31" s="33"/>
-      <c r="H31" s="1" t="s">
-        <v>34</v>
+      <c r="H31" s="1">
+        <v>2</v>
       </c>
       <c r="K31" s="28">
         <v>1</v>
@@ -2387,23 +2402,23 @@
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="20" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E32" s="8">
         <v>0</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G32" s="33"/>
-      <c r="H32" s="1" t="s">
-        <v>114</v>
+      <c r="H32" s="1">
+        <v>7</v>
       </c>
       <c r="K32" s="28">
         <v>1</v>
@@ -2421,23 +2436,23 @@
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E33" s="8">
         <v>0</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G33" s="33"/>
-      <c r="H33" s="1" t="s">
-        <v>4</v>
+      <c r="H33" s="1">
+        <v>1</v>
       </c>
       <c r="K33" s="28">
         <v>1</v>
@@ -2455,13 +2470,13 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="D34" s="1">
         <v>9</v>
@@ -2470,11 +2485,14 @@
         <v>1</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G34" s="33"/>
-      <c r="H34" s="1" t="s">
-        <v>123</v>
+      <c r="H34" s="1">
+        <v>3</v>
+      </c>
+      <c r="I34" s="7">
+        <v>8</v>
       </c>
       <c r="K34" s="28">
         <v>4</v>
@@ -2492,23 +2510,23 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E35" s="8">
         <v>0</v>
       </c>
       <c r="F35" s="36" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G35" s="37"/>
-      <c r="H35" s="15" t="s">
-        <v>114</v>
+      <c r="H35" s="15">
+        <v>7</v>
       </c>
       <c r="K35" s="28">
         <v>1</v>
@@ -2526,13 +2544,13 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D36" s="1">
         <v>9</v>
@@ -2541,45 +2559,45 @@
         <v>1</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G36" s="33"/>
-      <c r="H36" s="1" t="s">
-        <v>61</v>
+      <c r="H36" s="1">
+        <v>4</v>
       </c>
       <c r="K36" s="28">
         <v>1</v>
       </c>
-      <c r="L36" s="25">
+      <c r="L36" s="24">
         <v>1964</v>
       </c>
       <c r="M36" s="1">
         <v>2002</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O36" s="20"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E37" s="8">
         <v>0</v>
       </c>
       <c r="F37" s="33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G37" s="33"/>
-      <c r="H37" s="1" t="s">
-        <v>136</v>
+      <c r="H37" s="49">
+        <v>6</v>
       </c>
       <c r="K37" s="29"/>
       <c r="L37" s="1">
@@ -2595,13 +2613,13 @@
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D38" s="1">
         <v>9</v>
@@ -2610,11 +2628,11 @@
         <v>1</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G38" s="4"/>
-      <c r="H38" s="1" t="s">
-        <v>4</v>
+      <c r="H38" s="1">
+        <v>1</v>
       </c>
       <c r="K38" s="28">
         <v>1</v>
@@ -2632,12 +2650,12 @@
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="52" t="s">
         <v>25</v>
       </c>
       <c r="E39" s="8">
@@ -2647,8 +2665,8 @@
         <v>13</v>
       </c>
       <c r="G39" s="33"/>
-      <c r="H39" s="1" t="s">
-        <v>141</v>
+      <c r="J39" s="51" t="s">
+        <v>137</v>
       </c>
       <c r="K39" s="28">
         <v>1</v>
@@ -2666,13 +2684,13 @@
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E40" s="8">
         <v>0</v>
@@ -2681,8 +2699,8 @@
         <v>48</v>
       </c>
       <c r="G40" s="33"/>
-      <c r="H40" s="1" t="s">
-        <v>61</v>
+      <c r="H40" s="1">
+        <v>4</v>
       </c>
       <c r="K40" s="28">
         <v>1</v>
@@ -2700,33 +2718,33 @@
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D41" s="41" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
       <c r="H41" s="35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="41" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E42" s="41"/>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
       <c r="L42" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="M42" s="7"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K43" s="32"/>
       <c r="L43" s="45" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="M43" s="45"/>
     </row>
@@ -2797,18 +2815,200 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF96148D-3054-3446-B33B-11438D8AC45D}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="25">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B21" s="53"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="54"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B23" s="54"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B24" s="54"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B25" s="55"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B26" s="54"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B27" s="54"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B28" s="54"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B29" s="55"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B30" s="54"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B31" s="54"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B32" s="55"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B33" s="55"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="55"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B35" s="54"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B40" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069431B2-E190-0A4A-AD7A-67EB2654937C}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2821,6 +3021,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D51A4AB-EBA6-E24D-899D-2293B78CD359}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2831,16 +3032,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Moved data into 'rooms', 'subjects', & 'positions'
Moved subjects & positions into respective tables & added the 'rooms' table
</commit_message>
<xml_diff>
--- a/databases/staffDetails_L2.xlsx
+++ b/databases/staffDetails_L2.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tech/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA12A59-5649-2A40-956E-B2A66382B570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC5F1F-98C3-634D-BA74-51EEA23F862C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teachers" sheetId="1" r:id="rId1"/>
-    <sheet name="subjects" sheetId="4" r:id="rId2"/>
-    <sheet name="rooms" sheetId="3" r:id="rId3"/>
-    <sheet name="incomes" sheetId="2" r:id="rId4"/>
+    <sheet name="positions" sheetId="7" r:id="rId2"/>
+    <sheet name="subjects" sheetId="4" r:id="rId3"/>
+    <sheet name="departments" sheetId="6" r:id="rId4"/>
+    <sheet name="rooms" sheetId="3" r:id="rId5"/>
+    <sheet name="incomes" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="207">
   <si>
     <t>BRL</t>
   </si>
@@ -89,9 +91,6 @@
     <t>Fraser</t>
   </si>
   <si>
-    <t>Technology</t>
-  </si>
-  <si>
     <t>CTS</t>
   </si>
   <si>
@@ -635,13 +634,28 @@
     <t>Moved data to correct positon</t>
   </si>
   <si>
-    <t>HOD 1</t>
-  </si>
-  <si>
-    <t>HOD Digital 3</t>
-  </si>
-  <si>
     <t>Languages</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>hod_cypher</t>
+  </si>
+  <si>
+    <t>Digital Technology</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>Digital Technologies</t>
+  </si>
+  <si>
+    <t>position_name</t>
+  </si>
+  <si>
+    <t>HOD</t>
   </si>
 </sst>
 </file>
@@ -796,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -854,11 +868,13 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,8 +1195,8 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1190,7 +1206,7 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="4.1640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="31"/>
     <col min="13" max="13" width="14.5" style="10"/>
     <col min="15" max="15" width="3.33203125" customWidth="1"/>
@@ -1200,48 +1216,48 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="F1" s="43" t="s">
         <v>186</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>187</v>
       </c>
       <c r="G1" s="43"/>
       <c r="H1" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="J1" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="K1" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="L1" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="M1" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="N1" s="43" t="s">
         <v>193</v>
-      </c>
-      <c r="N1" s="43" t="s">
-        <v>194</v>
       </c>
       <c r="O1" s="43"/>
       <c r="Q1" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1260,8 +1276,8 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>3</v>
+      <c r="F2" s="33">
+        <v>8</v>
       </c>
       <c r="G2" s="33"/>
       <c r="H2" s="1">
@@ -1279,7 +1295,7 @@
       </c>
       <c r="O2" s="20"/>
       <c r="Q2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1295,8 +1311,8 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="38" t="s">
-        <v>153</v>
+      <c r="F3" s="38">
+        <v>20</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="1">
@@ -1316,7 +1332,7 @@
       </c>
       <c r="O3" s="20"/>
       <c r="Q3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1335,15 +1351,15 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>13</v>
+      <c r="F4" s="33">
+        <v>5</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="8">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
-        <v>158</v>
+      <c r="J4">
+        <v>1</v>
       </c>
       <c r="K4" s="28">
         <v>2</v>
@@ -1359,7 +1375,7 @@
       </c>
       <c r="O4" s="20"/>
       <c r="Q4" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1375,8 +1391,8 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="38" t="s">
-        <v>120</v>
+      <c r="F5" s="38">
+        <v>1</v>
       </c>
       <c r="G5" s="38"/>
       <c r="H5" s="1">
@@ -1396,18 +1412,18 @@
       </c>
       <c r="O5" s="20"/>
       <c r="Q5" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>12</v>
@@ -1415,8 +1431,8 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>22</v>
+      <c r="F6" s="33">
+        <v>21</v>
       </c>
       <c r="G6" s="33"/>
       <c r="H6" s="1">
@@ -1436,18 +1452,18 @@
       </c>
       <c r="O6" s="20"/>
       <c r="Q6" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>13</v>
@@ -1455,8 +1471,8 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>26</v>
+      <c r="F7" s="33">
+        <v>14</v>
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="8">
@@ -1479,31 +1495,31 @@
       </c>
       <c r="O7" s="20"/>
       <c r="Q7" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E8" s="8">
         <v>0</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>30</v>
+      <c r="F8" s="33">
+        <v>19</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="8">
         <v>2</v>
       </c>
-      <c r="J8" t="s">
-        <v>159</v>
+      <c r="J8">
+        <v>2</v>
       </c>
       <c r="K8" s="28">
         <v>5</v>
@@ -1519,18 +1535,18 @@
       </c>
       <c r="O8" s="20"/>
       <c r="Q8" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="1">
         <v>12</v>
@@ -1538,8 +1554,8 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="38" t="s">
-        <v>152</v>
+      <c r="F9" s="38">
+        <v>6</v>
       </c>
       <c r="G9" s="38"/>
       <c r="H9" s="1">
@@ -1559,18 +1575,18 @@
       </c>
       <c r="O9" s="20"/>
       <c r="Q9" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D10" s="1">
         <v>12</v>
@@ -1578,8 +1594,8 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="40" t="s">
-        <v>155</v>
+      <c r="F10" s="40">
+        <v>13</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="8">
@@ -1588,8 +1604,8 @@
       <c r="I10" s="7">
         <v>11</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>200</v>
+      <c r="J10" s="7">
+        <v>3</v>
       </c>
       <c r="K10" s="28">
         <v>2</v>
@@ -1605,18 +1621,18 @@
       </c>
       <c r="O10" s="20"/>
       <c r="Q10" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>11</v>
@@ -1624,8 +1640,8 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>41</v>
+      <c r="F11" s="33">
+        <v>18</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="1">
@@ -1645,24 +1661,24 @@
       </c>
       <c r="O11" s="20"/>
       <c r="Q11" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>44</v>
+      <c r="F12" s="33">
+        <v>2</v>
       </c>
       <c r="G12" s="33"/>
       <c r="H12" s="1">
@@ -1682,18 +1698,18 @@
       </c>
       <c r="O12" s="20"/>
       <c r="Q12" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D13" s="1">
         <v>10</v>
@@ -1701,15 +1717,15 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="33" t="s">
-        <v>48</v>
+      <c r="F13" s="33">
+        <v>9</v>
       </c>
       <c r="G13" s="33"/>
       <c r="H13" s="8">
         <v>4</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>201</v>
+      <c r="J13" s="57">
+        <v>3</v>
       </c>
       <c r="K13" s="30">
         <v>2</v>
@@ -1725,31 +1741,31 @@
       </c>
       <c r="O13" s="20"/>
       <c r="Q13" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>13</v>
+      <c r="F14" s="33">
+        <v>5</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="8">
         <v>1</v>
       </c>
-      <c r="J14" t="s">
-        <v>164</v>
+      <c r="J14">
+        <v>4</v>
       </c>
       <c r="K14" s="28">
         <v>6</v>
@@ -1765,18 +1781,18 @@
       </c>
       <c r="O14" s="20"/>
       <c r="Q14" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="1">
         <v>11</v>
@@ -1784,8 +1800,8 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="33" t="s">
-        <v>54</v>
+      <c r="F15" s="33">
+        <v>10</v>
       </c>
       <c r="G15" s="33"/>
       <c r="H15" s="1">
@@ -1805,18 +1821,18 @@
       </c>
       <c r="O15" s="20"/>
       <c r="Q15" s="50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D16" s="1">
         <v>13</v>
@@ -1824,8 +1840,8 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="40" t="s">
-        <v>26</v>
+      <c r="F16" s="40">
+        <v>14</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="1">
@@ -1847,13 +1863,13 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D17" s="1">
         <v>12</v>
@@ -1861,8 +1877,8 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="33" t="s">
-        <v>54</v>
+      <c r="F17" s="33">
+        <v>10</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="1">
@@ -1884,26 +1900,26 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E18" s="8">
         <v>0</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>65</v>
+      <c r="F18" s="33">
+        <v>16</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="8">
         <v>2</v>
       </c>
-      <c r="J18" t="s">
-        <v>165</v>
+      <c r="J18">
+        <v>5</v>
       </c>
       <c r="K18" s="28">
         <v>5</v>
@@ -1921,13 +1937,13 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D19" s="1">
         <v>12</v>
@@ -1935,8 +1951,8 @@
       <c r="E19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" s="38" t="s">
-        <v>100</v>
+      <c r="F19" s="38">
+        <v>15</v>
       </c>
       <c r="G19" s="38"/>
       <c r="H19" s="1">
@@ -1958,19 +1974,19 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E20" s="8">
         <v>0</v>
       </c>
-      <c r="F20" s="38" t="s">
-        <v>151</v>
+      <c r="F20" s="38">
+        <v>25</v>
       </c>
       <c r="G20" s="38"/>
       <c r="H20" s="1">
@@ -1992,19 +2008,19 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E21" s="8">
         <v>0</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>13</v>
+      <c r="F21" s="33">
+        <v>5</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="2"/>
@@ -2024,13 +2040,13 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D22" s="1">
         <v>11</v>
@@ -2038,8 +2054,8 @@
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="F22" s="33" t="s">
-        <v>78</v>
+      <c r="F22" s="33">
+        <v>7</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="47">
@@ -2062,13 +2078,13 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D23" s="1">
         <v>10</v>
@@ -2076,8 +2092,8 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="38" t="s">
-        <v>152</v>
+      <c r="F23" s="38">
+        <v>6</v>
       </c>
       <c r="G23" s="39"/>
       <c r="H23" s="8">
@@ -2102,26 +2118,26 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E24" s="8">
         <v>0</v>
       </c>
-      <c r="F24" s="33" t="s">
-        <v>13</v>
+      <c r="F24" s="33">
+        <v>5</v>
       </c>
       <c r="G24" s="33"/>
       <c r="H24" s="8">
         <v>4</v>
       </c>
-      <c r="J24" t="s">
-        <v>167</v>
+      <c r="J24">
+        <v>6</v>
       </c>
       <c r="K24" s="28">
         <v>6</v>
@@ -2139,13 +2155,13 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D25" s="1">
         <v>10</v>
@@ -2153,8 +2169,8 @@
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="33" t="s">
-        <v>88</v>
+      <c r="F25" s="33">
+        <v>12</v>
       </c>
       <c r="G25" s="33"/>
       <c r="H25" s="8">
@@ -2179,19 +2195,19 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E26" s="8">
         <v>0</v>
       </c>
-      <c r="F26" s="33" t="s">
-        <v>92</v>
+      <c r="F26" s="33">
+        <v>24</v>
       </c>
       <c r="G26" s="33"/>
       <c r="H26" s="8">
@@ -2200,8 +2216,8 @@
       <c r="I26" s="7">
         <v>10</v>
       </c>
-      <c r="J26" t="s">
-        <v>168</v>
+      <c r="J26">
+        <v>7</v>
       </c>
       <c r="K26" s="28">
         <v>7</v>
@@ -2219,13 +2235,13 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D27" s="1">
         <v>9</v>
@@ -2233,8 +2249,8 @@
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>96</v>
+      <c r="F27" s="33">
+        <v>17</v>
       </c>
       <c r="G27" s="33"/>
       <c r="H27" s="1">
@@ -2254,13 +2270,13 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
@@ -2268,8 +2284,8 @@
       <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="33" t="s">
-        <v>100</v>
+      <c r="F28" s="33">
+        <v>15</v>
       </c>
       <c r="G28" s="33"/>
       <c r="H28" s="8">
@@ -2291,19 +2307,19 @@
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="E29" s="8">
         <v>0</v>
       </c>
-      <c r="F29" s="33" t="s">
-        <v>102</v>
+      <c r="F29" s="33">
+        <v>4</v>
       </c>
       <c r="G29" s="33"/>
       <c r="H29" s="49">
@@ -2325,13 +2341,13 @@
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C30" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30" s="1">
         <v>12</v>
@@ -2339,8 +2355,8 @@
       <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="33" t="s">
-        <v>105</v>
+      <c r="F30" s="33">
+        <v>23</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="8">
@@ -2365,13 +2381,13 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="D31" s="1">
         <v>10</v>
@@ -2379,8 +2395,8 @@
       <c r="E31" s="1">
         <v>1</v>
       </c>
-      <c r="F31" s="33" t="s">
-        <v>30</v>
+      <c r="F31" s="33">
+        <v>19</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="1">
@@ -2402,24 +2418,27 @@
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="E32" s="8">
         <v>0</v>
       </c>
-      <c r="F32" s="33" t="s">
-        <v>111</v>
+      <c r="F32" s="33">
+        <v>26</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="1">
         <v>7</v>
       </c>
+      <c r="I32" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="K32" s="28">
         <v>1</v>
       </c>
@@ -2436,19 +2455,19 @@
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="E33" s="8">
         <v>0</v>
       </c>
-      <c r="F33" s="33" t="s">
-        <v>116</v>
+      <c r="F33" s="33">
+        <v>22</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="1">
@@ -2470,13 +2489,13 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D34" s="1">
         <v>9</v>
@@ -2484,8 +2503,8 @@
       <c r="E34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="33" t="s">
-        <v>120</v>
+      <c r="F34" s="33">
+        <v>1</v>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="1">
@@ -2510,19 +2529,19 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="E35" s="8">
         <v>0</v>
       </c>
-      <c r="F35" s="36" t="s">
-        <v>170</v>
+      <c r="F35" s="36">
+        <v>27</v>
       </c>
       <c r="G35" s="37"/>
       <c r="H35" s="15">
@@ -2544,13 +2563,13 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="D36" s="1">
         <v>9</v>
@@ -2558,8 +2577,8 @@
       <c r="E36" s="1">
         <v>1</v>
       </c>
-      <c r="F36" s="33" t="s">
-        <v>127</v>
+      <c r="F36" s="33">
+        <v>11</v>
       </c>
       <c r="G36" s="33"/>
       <c r="H36" s="1">
@@ -2575,25 +2594,25 @@
         <v>2002</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O36" s="20"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E37" s="8">
         <v>0</v>
       </c>
-      <c r="F37" s="33" t="s">
-        <v>132</v>
+      <c r="F37" s="33">
+        <v>3</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="49">
@@ -2613,13 +2632,13 @@
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D38" s="1">
         <v>9</v>
@@ -2627,8 +2646,8 @@
       <c r="E38" s="1">
         <v>1</v>
       </c>
-      <c r="F38" s="9" t="s">
-        <v>116</v>
+      <c r="F38" s="9">
+        <v>22</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="1">
@@ -2650,23 +2669,23 @@
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="C39" s="52" t="s">
-        <v>25</v>
+        <v>135</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="E39" s="8">
         <v>0</v>
       </c>
-      <c r="F39" s="33" t="s">
-        <v>13</v>
+      <c r="F39" s="33">
+        <v>5</v>
       </c>
       <c r="G39" s="33"/>
-      <c r="J39" s="51" t="s">
-        <v>137</v>
+      <c r="J39" s="56">
+        <v>8</v>
       </c>
       <c r="K39" s="28">
         <v>1</v>
@@ -2684,19 +2703,19 @@
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E40" s="8">
         <v>0</v>
       </c>
-      <c r="F40" s="33" t="s">
-        <v>48</v>
+      <c r="F40" s="33">
+        <v>9</v>
       </c>
       <c r="G40" s="33"/>
       <c r="H40" s="1">
@@ -2718,33 +2737,33 @@
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D41" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
       <c r="H41" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42" s="41"/>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
       <c r="L42" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M42" s="7"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K43" s="32"/>
       <c r="L43" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M43" s="45"/>
     </row>
@@ -2814,192 +2833,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF96148D-3054-3446-B33B-11438D8AC45D}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB89868C-F4B5-6D49-BCC9-A125C79DF23B}">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>4</v>
+      <c r="B2" s="25" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>34</v>
+      <c r="B3" s="25" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
+      <c r="B4" s="25" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="25">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>161</v>
+      <c r="B6" s="25" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="25">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>198</v>
+      <c r="B7" s="25" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="25">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>112</v>
+      <c r="B8" s="25" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="25">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>166</v>
+      <c r="B9" s="56" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="25">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>202</v>
-      </c>
+      <c r="B10" s="25"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="25">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="25">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>162</v>
-      </c>
+      <c r="B11" s="55"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B13" s="25"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B14" s="8"/>
+      <c r="B14" s="25"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B16" s="8"/>
+      <c r="B15" s="25"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B17" s="8"/>
+      <c r="B17" s="25"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B18" s="8"/>
+      <c r="B18" s="25"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B19" s="8"/>
+      <c r="B19" s="25"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B20" s="8"/>
+      <c r="B20" s="25"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B21" s="53"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B22" s="54"/>
+      <c r="B21" s="25"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B23" s="54"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B24" s="54"/>
+      <c r="B23" s="25"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B25" s="55"/>
+      <c r="B25" s="25"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B26" s="54"/>
+      <c r="B26" s="25"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B27" s="54"/>
+      <c r="B27" s="25"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B28" s="54"/>
+      <c r="B28" s="25"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B29" s="55"/>
+      <c r="B29" s="25"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B30" s="54"/>
+      <c r="B30" s="25"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B31" s="54"/>
+      <c r="B31" s="25"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B32" s="55"/>
+      <c r="B32" s="25"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B33" s="55"/>
+      <c r="B33" s="25"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B34" s="55"/>
+      <c r="B34" s="25"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B35" s="54"/>
+      <c r="B35" s="25"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B36" s="8"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B38" s="8"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B40" s="8"/>
+      <c r="B36" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3007,19 +2992,558 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069431B2-E190-0A4A-AD7A-67EB2654937C}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF96148D-3054-3446-B33B-11438D8AC45D}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="25">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B21" s="52"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="53"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B23" s="53"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B24" s="53"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B25" s="54"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B26" s="53"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B27" s="53"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B28" s="53"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B29" s="54"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B30" s="53"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B31" s="53"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B32" s="54"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B33" s="54"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="54"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B35" s="53"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B40" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D667F3-E611-D947-8C57-ECFC36D620AB}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069431B2-E190-0A4A-AD7A-67EB2654937C}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="25"/>
+    <col min="3" max="3" width="10.83203125" style="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="57"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="57"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="57"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="57"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="57"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="57"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="57"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="25">
+        <v>8</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="57"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="57"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="57"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="57"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="57"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="25">
+        <v>13</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="57"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="25">
+        <v>14</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="57"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="25">
+        <v>15</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="57"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="25">
+        <v>16</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="57"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="25">
+        <v>17</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="57"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="25">
+        <v>18</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="57"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="25">
+        <v>19</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="57"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="25">
+        <v>20</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="57"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="25">
+        <v>21</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="57"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="25">
+        <v>22</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="57"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="25">
+        <v>23</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="57"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="57"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="25">
+        <v>25</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="57"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="25">
+        <v>26</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="57"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="25">
+        <v>27</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="57"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C32">
+    <sortCondition ref="B2:B32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D51A4AB-EBA6-E24D-899D-2293B78CD359}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D8"/>
@@ -3032,16 +3556,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>195</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Changed some field formatting
Changed field sizes and renamed `teachers`.`room`to `teachers`.`room_id`
</commit_message>
<xml_diff>
--- a/databases/staffDetails_L2.xlsx
+++ b/databases/staffDetails_L2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tech/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC5F1F-98C3-634D-BA74-51EEA23F862C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382C609C-26BC-3C46-9DE2-C46344920D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1195,8 +1195,8 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16:G16"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1205,10 +1205,12 @@
     <col min="4" max="5" width="22.1640625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="4.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="31"/>
-    <col min="13" max="13" width="14.5" style="10"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="10" customWidth="1"/>
     <col min="15" max="15" width="3.33203125" customWidth="1"/>
     <col min="17" max="17" width="40.83203125" customWidth="1"/>
     <col min="18" max="18" width="20.1640625" customWidth="1"/>

</xml_diff>

<commit_message>
Made slight changes to table
</commit_message>
<xml_diff>
--- a/databases/staffDetails_L2.xlsx
+++ b/databases/staffDetails_L2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16515"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16515" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="teachers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="237">
   <si>
     <t>BRL</t>
   </si>
@@ -581,18 +581,12 @@
     <t>teacher_cypher</t>
   </si>
   <si>
-    <t>theacher_christan</t>
-  </si>
-  <si>
     <t>teacher_form</t>
   </si>
   <si>
     <t>teacher_form_mentors</t>
   </si>
   <si>
-    <t>room</t>
-  </si>
-  <si>
     <t>subject</t>
   </si>
   <si>
@@ -632,9 +626,6 @@
     <t>Digital Technology</t>
   </si>
   <si>
-    <t>department</t>
-  </si>
-  <si>
     <t>position_name</t>
   </si>
   <si>
@@ -750,6 +741,9 @@
   </si>
   <si>
     <t>HOD_Digital Technologies</t>
+  </si>
+  <si>
+    <t>teacher_christan</t>
   </si>
 </sst>
 </file>
@@ -954,23 +948,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1290,9 +1284,9 @@
   </sheetPr>
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1320,37 +1314,37 @@
         <v>180</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="G1" s="49"/>
+      <c r="H1" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="I1" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="35" t="s">
+      <c r="J1" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="K1" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="L1" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="M1" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="L1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="M1" s="51" t="s">
-        <v>191</v>
-      </c>
-      <c r="N1" s="51"/>
+      <c r="N1" s="49"/>
       <c r="P1" s="8" t="s">
         <v>149</v>
       </c>
@@ -1366,15 +1360,15 @@
         <v>2</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2" s="52">
+        <v>220</v>
+      </c>
+      <c r="F2" s="50">
         <v>8</v>
       </c>
-      <c r="G2" s="52"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="1">
         <v>1</v>
       </c>
@@ -1403,10 +1397,10 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="55">
         <v>20</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="1">
         <v>1</v>
       </c>
@@ -1438,13 +1432,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4" s="34"/>
-      <c r="F4" s="52">
+      <c r="F4" s="50">
         <v>5</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="8">
         <v>2</v>
       </c>
@@ -1479,10 +1473,10 @@
         <v>17</v>
       </c>
       <c r="E5" s="34"/>
-      <c r="F5" s="53">
-        <v>1</v>
-      </c>
-      <c r="G5" s="53"/>
+      <c r="F5" s="55">
+        <v>1</v>
+      </c>
+      <c r="G5" s="55"/>
       <c r="H5" s="1">
         <v>3</v>
       </c>
@@ -1514,13 +1508,13 @@
         <v>20</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="52">
+      <c r="F6" s="50">
         <v>21</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="50"/>
       <c r="H6" s="1">
         <v>1</v>
       </c>
@@ -1552,13 +1546,13 @@
         <v>24</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E7" s="34"/>
-      <c r="F7" s="52">
+      <c r="F7" s="50">
         <v>14</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="8">
         <v>1</v>
       </c>
@@ -1590,10 +1584,10 @@
         <v>28</v>
       </c>
       <c r="E8" s="34"/>
-      <c r="F8" s="52">
+      <c r="F8" s="50">
         <v>19</v>
       </c>
-      <c r="G8" s="52"/>
+      <c r="G8" s="50"/>
       <c r="H8" s="8">
         <v>2</v>
       </c>
@@ -1628,13 +1622,13 @@
         <v>32</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E9" s="34"/>
-      <c r="F9" s="53">
+      <c r="F9" s="55">
         <v>6</v>
       </c>
-      <c r="G9" s="53"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="1">
         <v>2</v>
       </c>
@@ -1666,13 +1660,13 @@
         <v>36</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E10" s="34"/>
-      <c r="F10" s="54">
+      <c r="F10" s="57">
         <v>13</v>
       </c>
-      <c r="G10" s="54"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="8">
         <v>1</v>
       </c>
@@ -1707,13 +1701,13 @@
         <v>39</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E11" s="34"/>
-      <c r="F11" s="52">
+      <c r="F11" s="50">
         <v>18</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="1">
         <v>2</v>
       </c>
@@ -1745,10 +1739,10 @@
         <v>148</v>
       </c>
       <c r="E12" s="34"/>
-      <c r="F12" s="52">
+      <c r="F12" s="50">
         <v>2</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="1">
         <v>3</v>
       </c>
@@ -1780,15 +1774,15 @@
         <v>46</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F13" s="52">
+        <v>221</v>
+      </c>
+      <c r="F13" s="50">
         <v>9</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="8">
         <v>4</v>
       </c>
@@ -1823,10 +1817,10 @@
         <v>50</v>
       </c>
       <c r="E14" s="34"/>
-      <c r="F14" s="52">
+      <c r="F14" s="50">
         <v>5</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="8">
         <v>1</v>
       </c>
@@ -1861,13 +1855,13 @@
         <v>146</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E15" s="34"/>
-      <c r="F15" s="52">
+      <c r="F15" s="50">
         <v>10</v>
       </c>
-      <c r="G15" s="52"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="1">
         <v>1</v>
       </c>
@@ -1885,7 +1879,7 @@
       </c>
       <c r="N15" s="20"/>
       <c r="P15" s="41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1899,13 +1893,13 @@
         <v>56</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E16" s="34"/>
-      <c r="F16" s="54">
+      <c r="F16" s="57">
         <v>14</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="1">
         <v>1</v>
       </c>
@@ -1934,13 +1928,13 @@
         <v>59</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E17" s="34"/>
-      <c r="F17" s="52">
+      <c r="F17" s="50">
         <v>10</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="1">
         <v>4</v>
       </c>
@@ -1969,10 +1963,10 @@
         <v>63</v>
       </c>
       <c r="E18" s="34"/>
-      <c r="F18" s="52">
+      <c r="F18" s="50">
         <v>16</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="50"/>
       <c r="H18" s="8">
         <v>2</v>
       </c>
@@ -2004,13 +1998,13 @@
         <v>67</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E19" s="34"/>
-      <c r="F19" s="53">
+      <c r="F19" s="55">
         <v>15</v>
       </c>
-      <c r="G19" s="53"/>
+      <c r="G19" s="55"/>
       <c r="H19" s="1">
         <v>2</v>
       </c>
@@ -2039,10 +2033,10 @@
         <v>70</v>
       </c>
       <c r="E20" s="34"/>
-      <c r="F20" s="53">
+      <c r="F20" s="55">
         <v>25</v>
       </c>
-      <c r="G20" s="53"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="1">
         <v>1</v>
       </c>
@@ -2071,10 +2065,10 @@
         <v>73</v>
       </c>
       <c r="E21" s="34"/>
-      <c r="F21" s="52">
+      <c r="F21" s="50">
         <v>5</v>
       </c>
-      <c r="G21" s="52"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="2"/>
       <c r="J21" s="28">
         <v>3</v>
@@ -2101,13 +2095,13 @@
         <v>76</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E22" s="34"/>
-      <c r="F22" s="52">
+      <c r="F22" s="50">
         <v>7</v>
       </c>
-      <c r="G22" s="52"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="39">
         <v>2</v>
       </c>
@@ -2136,15 +2130,15 @@
         <v>80</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F23" s="53">
+        <v>222</v>
+      </c>
+      <c r="F23" s="55">
         <v>6</v>
       </c>
-      <c r="G23" s="55"/>
+      <c r="G23" s="56"/>
       <c r="H23" s="8">
         <v>1</v>
       </c>
@@ -2173,10 +2167,10 @@
         <v>83</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="52">
+      <c r="F24" s="50">
         <v>5</v>
       </c>
-      <c r="G24" s="52"/>
+      <c r="G24" s="50"/>
       <c r="H24" s="8">
         <v>4</v>
       </c>
@@ -2208,15 +2202,15 @@
         <v>86</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F25" s="52">
+        <v>223</v>
+      </c>
+      <c r="F25" s="50">
         <v>12</v>
       </c>
-      <c r="G25" s="52"/>
+      <c r="G25" s="50"/>
       <c r="H25" s="8">
         <v>1</v>
       </c>
@@ -2245,10 +2239,10 @@
         <v>90</v>
       </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="52">
+      <c r="F26" s="50">
         <v>24</v>
       </c>
-      <c r="G26" s="52"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="8">
         <v>2</v>
       </c>
@@ -2280,15 +2274,15 @@
         <v>94</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F27" s="52">
+        <v>224</v>
+      </c>
+      <c r="F27" s="50">
         <v>17</v>
       </c>
-      <c r="G27" s="52"/>
+      <c r="G27" s="50"/>
       <c r="H27" s="1">
         <v>2</v>
       </c>
@@ -2315,15 +2309,15 @@
         <v>98</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F28" s="52">
+        <v>225</v>
+      </c>
+      <c r="F28" s="50">
         <v>15</v>
       </c>
-      <c r="G28" s="52"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="8">
         <v>2</v>
       </c>
@@ -2352,10 +2346,10 @@
         <v>145</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="52">
+      <c r="F29" s="50">
         <v>4</v>
       </c>
-      <c r="G29" s="52"/>
+      <c r="G29" s="50"/>
       <c r="H29" s="40">
         <v>6</v>
       </c>
@@ -2384,13 +2378,13 @@
         <v>122</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="52">
+      <c r="F30" s="50">
         <v>23</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="50"/>
       <c r="H30" s="8">
         <v>1</v>
       </c>
@@ -2419,15 +2413,15 @@
         <v>107</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F31" s="52">
+        <v>226</v>
+      </c>
+      <c r="F31" s="50">
         <v>19</v>
       </c>
-      <c r="G31" s="52"/>
+      <c r="G31" s="50"/>
       <c r="H31" s="1">
         <v>2</v>
       </c>
@@ -2456,10 +2450,10 @@
         <v>109</v>
       </c>
       <c r="E32" s="8"/>
-      <c r="F32" s="52">
+      <c r="F32" s="50">
         <v>26</v>
       </c>
-      <c r="G32" s="52"/>
+      <c r="G32" s="50"/>
       <c r="H32" s="1">
         <v>7</v>
       </c>
@@ -2488,10 +2482,10 @@
         <v>114</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="52">
+      <c r="F33" s="50">
         <v>22</v>
       </c>
-      <c r="G33" s="52"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="1">
         <v>1</v>
       </c>
@@ -2520,15 +2514,15 @@
         <v>118</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F34" s="52">
-        <v>1</v>
-      </c>
-      <c r="G34" s="52"/>
+        <v>227</v>
+      </c>
+      <c r="F34" s="50">
+        <v>1</v>
+      </c>
+      <c r="G34" s="50"/>
       <c r="H34" s="1">
         <v>3</v>
       </c>
@@ -2557,10 +2551,10 @@
         <v>122</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="58">
+      <c r="F35" s="52">
         <v>27</v>
       </c>
-      <c r="G35" s="59"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="15">
         <v>7</v>
       </c>
@@ -2589,15 +2583,15 @@
         <v>125</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F36" s="52">
+        <v>228</v>
+      </c>
+      <c r="F36" s="50">
         <v>11</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="50"/>
       <c r="H36" s="1">
         <v>4</v>
       </c>
@@ -2626,10 +2620,10 @@
         <v>130</v>
       </c>
       <c r="E37" s="8"/>
-      <c r="F37" s="52">
+      <c r="F37" s="50">
         <v>3</v>
       </c>
-      <c r="G37" s="52"/>
+      <c r="G37" s="50"/>
       <c r="H37" s="40">
         <v>6</v>
       </c>
@@ -2656,10 +2650,10 @@
         <v>134</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F38" s="9">
         <v>22</v>
@@ -2693,10 +2687,10 @@
         <v>24</v>
       </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="52">
+      <c r="F39" s="50">
         <v>5</v>
       </c>
-      <c r="G39" s="52"/>
+      <c r="G39" s="50"/>
       <c r="I39" s="47">
         <v>8</v>
       </c>
@@ -2725,10 +2719,10 @@
         <v>138</v>
       </c>
       <c r="E40" s="8"/>
-      <c r="F40" s="52">
+      <c r="F40" s="50">
         <v>9</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="50"/>
       <c r="H40" s="1">
         <v>4</v>
       </c>
@@ -2747,24 +2741,24 @@
       <c r="N40" s="20"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D41" s="50" t="s">
+      <c r="D41" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="50"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="57" t="s">
+      <c r="E41" s="59"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="I41" s="57"/>
+      <c r="I41" s="54"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D42" s="50" t="s">
+      <c r="D42" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="E42" s="50"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
       <c r="K42" s="7" t="s">
         <v>173</v>
       </c>
@@ -2772,25 +2766,55 @@
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J43" s="32"/>
-      <c r="K43" s="49" t="s">
+      <c r="K43" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="L43" s="49"/>
+      <c r="L43" s="58"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
     </row>
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K46" s="49"/>
-      <c r="L46" s="49"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="K43:L46"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
@@ -2807,36 +2831,6 @@
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K43:L46"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2848,21 +2842,19 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>199</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -2871,9 +2863,7 @@
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -2888,11 +2878,9 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C4" s="7">
-        <v>2</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="25">
@@ -2915,7 +2903,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2939,7 +2927,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3059,10 +3047,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3086,7 +3074,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3134,7 +3122,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3213,7 +3201,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G46" sqref="G46:G48"/>
     </sheetView>
   </sheetViews>
@@ -3225,10 +3213,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3491,7 +3479,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3499,16 +3487,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>